<commit_message>
Fixed errors in tables
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik Gustafsson\Documents\Skolarbete\Uppsats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik Gustafsson\Documents\Skolarbete\Uppsats\OpenAI-Feedback-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DE94E2-F894-4760-9AFD-9D1D01219D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD01349B-79A0-424D-A99A-AF214053E174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="1455" windowWidth="21600" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28005" yWindow="0" windowWidth="23595" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,26 +222,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,35 +534,35 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
       <c r="O3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="O4" t="s">
@@ -575,10 +574,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>0.5</v>
@@ -638,10 +637,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -658,10 +657,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -747,10 +746,10 @@
         <v>15</v>
       </c>
       <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
         <v>0.5</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -794,14 +793,14 @@
       </c>
       <c r="C15" s="1">
         <f>SUM(C5:C14)</f>
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
+        <f>SUM(D5:D14)</f>
         <v>6</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" ref="D15:L15" si="0">SUM(D5:D14)</f>
-        <v>4</v>
-      </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D15:G15" si="0">SUM(E5:E14)</f>
         <v>8</v>
       </c>
       <c r="F15" s="1">
@@ -817,54 +816,54 @@
       <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="2">
-        <f>SUM(C15:G15)</f>
-        <v>30</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="C16" s="9">
+        <f>SUM(D15:G15)</f>
+        <v>26</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="2">
-        <f>AVERAGE(C5:G14)</f>
-        <v>0.6</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="C17" s="9">
+        <f>AVERAGE(D5:G14)</f>
+        <v>0.65</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -873,10 +872,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -965,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -993,10 +992,10 @@
         <v>13</v>
       </c>
       <c r="C28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -1039,7 +1038,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F30" s="1">
         <v>0.5</v>
@@ -1053,10 +1052,10 @@
         <v>16</v>
       </c>
       <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
         <v>0.5</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -1074,15 +1073,15 @@
       </c>
       <c r="C32" s="1">
         <f>SUM(C22:C31)</f>
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="D32" s="1">
         <f>SUM(D22:D31)</f>
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="E32" s="1">
         <f>SUM(E22:E31)</f>
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="F32" s="1">
         <f>SUM(F22:F31)</f>
@@ -1090,43 +1089,43 @@
       </c>
       <c r="G32" s="1">
         <f>SUM(G22:G31)</f>
-        <v>7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="9">
         <f>SUM(C32:G32)</f>
         <v>42</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="9">
         <f>AVERAGE(C22:G31)</f>
         <v>0.84</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C34:G34"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="C33:G33"/>
     <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>